<commit_message>
pensando en automatizar protocolos para crear archivos correspondientes a diferentes examenes
</commit_message>
<xml_diff>
--- a/docs/PROCEDIMIENTOS.xlsx
+++ b/docs/PROCEDIMIENTOS.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CURSOS\Python\mini_projects\MecanOdei\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84383775-3AAD-4B01-B991-7D1E4CA6AA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="105" windowWidth="14055" windowHeight="8970"/>
+    <workbookView xWindow="-28920" yWindow="1860" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -240,8 +246,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -523,67 +529,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -591,42 +549,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -673,7 +683,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -705,9 +715,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -739,6 +767,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -914,18 +960,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="32" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="16" customWidth="1"/>
     <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -933,59 +979,59 @@
     <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
-      <c r="G1" s="44" t="s">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7">
-        <v>1</v>
-      </c>
-      <c r="J2" s="7">
-        <v>1</v>
-      </c>
-      <c r="K2" s="39">
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5">
+        <v>1</v>
+      </c>
+      <c r="K2" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="12"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
       <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="34"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4">
@@ -994,21 +1040,21 @@
       <c r="J3" s="4">
         <v>1</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="12"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="22"/>
       <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="34"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4">
         <v>1</v>
@@ -1019,75 +1065,75 @@
       <c r="J4" s="4">
         <v>2</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="8">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15">
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
+      <c r="B5" s="9">
         <v>4</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="31" t="s">
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="15">
-        <v>1</v>
-      </c>
-      <c r="H5" s="15">
-        <v>1</v>
-      </c>
-      <c r="I5" s="15">
-        <v>2</v>
-      </c>
-      <c r="J5" s="15">
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>2</v>
+      </c>
+      <c r="J5" s="9">
         <v>3</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="10">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="10" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9">
-        <v>1</v>
-      </c>
-      <c r="J6" s="9">
-        <v>1</v>
-      </c>
-      <c r="K6" s="11">
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="12"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
       <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="34"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4">
@@ -1096,21 +1142,21 @@
       <c r="J7" s="4">
         <v>1</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="12"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
       <c r="B8" s="4">
         <v>3</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="34" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="4"/>
@@ -1123,73 +1169,73 @@
       <c r="J8" s="4">
         <v>2</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="8">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
+      <c r="B9" s="9">
         <v>4</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="31" t="s">
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="15">
-        <v>1</v>
-      </c>
-      <c r="H9" s="15">
-        <v>1</v>
-      </c>
-      <c r="I9" s="15">
-        <v>2</v>
-      </c>
-      <c r="J9" s="15">
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>2</v>
+      </c>
+      <c r="J9" s="9">
         <v>3</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="10">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-      <c r="C10" s="10" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9">
-        <v>1</v>
-      </c>
-      <c r="K10" s="11">
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6">
+        <v>1</v>
+      </c>
+      <c r="K10" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
       <c r="B11" s="4">
         <v>2</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="34"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4">
@@ -1198,21 +1244,21 @@
       <c r="J11" s="4">
         <v>1</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="12"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
       <c r="B12" s="4">
         <v>3</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="34"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="3"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4">
         <v>1</v>
@@ -1223,73 +1269,73 @@
       <c r="J12" s="4">
         <v>2</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15">
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
+      <c r="B13" s="9">
         <v>4</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="31" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="15">
-        <v>1</v>
-      </c>
-      <c r="H13" s="15">
-        <v>1</v>
-      </c>
-      <c r="I13" s="15">
-        <v>2</v>
-      </c>
-      <c r="J13" s="15">
+      <c r="G13" s="9">
+        <v>1</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9">
+        <v>2</v>
+      </c>
+      <c r="J13" s="9">
         <v>3</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="10">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="8" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="9">
-        <v>1</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9">
-        <v>1</v>
-      </c>
-      <c r="K14" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="12"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6">
+        <v>1</v>
+      </c>
+      <c r="K14" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
       <c r="B15" s="4">
         <v>2</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="34"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4">
@@ -1298,21 +1344,21 @@
       <c r="J15" s="4">
         <v>1</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="12"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
       <c r="B16" s="4">
         <v>3</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="34"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4">
         <v>1</v>
@@ -1323,109 +1369,109 @@
       <c r="J16" s="4">
         <v>2</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="8">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="9">
         <v>4</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="17"/>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="18" t="s">
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="9">
-        <v>1</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9">
-        <v>1</v>
-      </c>
-      <c r="K18" s="11">
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6">
+        <v>1</v>
+      </c>
+      <c r="K18" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A19" s="19"/>
-      <c r="B19" s="15">
-        <v>2</v>
-      </c>
-      <c r="C19" s="16" t="s">
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26"/>
+      <c r="B19" s="9">
+        <v>2</v>
+      </c>
+      <c r="C19" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15">
-        <v>1</v>
-      </c>
-      <c r="J19" s="15">
-        <v>1</v>
-      </c>
-      <c r="K19" s="17">
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9">
+        <v>1</v>
+      </c>
+      <c r="J19" s="9">
+        <v>1</v>
+      </c>
+      <c r="K19" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="9">
-        <v>1</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9">
-        <v>1</v>
-      </c>
-      <c r="J20" s="9">
-        <v>1</v>
-      </c>
-      <c r="K20" s="11">
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6">
+        <v>1</v>
+      </c>
+      <c r="J20" s="6">
+        <v>1</v>
+      </c>
+      <c r="K20" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="20"/>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
       <c r="B21" s="4">
         <v>2</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="34"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="3"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4">
         <v>1</v>
@@ -1436,75 +1482,75 @@
       <c r="J21" s="4">
         <v>2</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K21" s="8">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="15">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="26"/>
+      <c r="B22" s="9">
         <v>3</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="15">
-        <v>1</v>
-      </c>
-      <c r="H22" s="15">
-        <v>1</v>
-      </c>
-      <c r="I22" s="15">
-        <v>2</v>
-      </c>
-      <c r="J22" s="15">
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="9">
+        <v>1</v>
+      </c>
+      <c r="H22" s="9">
+        <v>1</v>
+      </c>
+      <c r="I22" s="9">
+        <v>2</v>
+      </c>
+      <c r="J22" s="9">
         <v>3</v>
       </c>
-      <c r="K22" s="17">
+      <c r="K22" s="10">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="9">
-        <v>1</v>
-      </c>
-      <c r="C23" s="10" t="s">
+      <c r="B23" s="6">
+        <v>1</v>
+      </c>
+      <c r="C23" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="21" t="s">
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9">
-        <v>1</v>
-      </c>
-      <c r="J23" s="9">
-        <v>1</v>
-      </c>
-      <c r="K23" s="11">
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6">
+        <v>1</v>
+      </c>
+      <c r="J23" s="6">
+        <v>1</v>
+      </c>
+      <c r="K23" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="12"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="22"/>
       <c r="B24" s="4">
         <v>2</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="3"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="42"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4">
@@ -1513,21 +1559,21 @@
       <c r="J24" s="4">
         <v>2</v>
       </c>
-      <c r="K24" s="13">
+      <c r="K24" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="12"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
       <c r="B25" s="4">
         <v>3</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="3"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="42"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4">
         <v>1</v>
@@ -1538,73 +1584,73 @@
       <c r="J25" s="4">
         <v>3</v>
       </c>
-      <c r="K25" s="13">
+      <c r="K25" s="8">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="23"/>
+      <c r="B26" s="9">
         <v>4</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="31" t="s">
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="15">
-        <v>1</v>
-      </c>
-      <c r="H26" s="15">
-        <v>1</v>
-      </c>
-      <c r="I26" s="15">
+      <c r="G26" s="9">
+        <v>1</v>
+      </c>
+      <c r="H26" s="9">
+        <v>1</v>
+      </c>
+      <c r="I26" s="9">
         <v>3</v>
       </c>
-      <c r="J26" s="15">
+      <c r="J26" s="9">
         <v>6</v>
       </c>
-      <c r="K26" s="17">
+      <c r="K26" s="10">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="18" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="9">
-        <v>1</v>
-      </c>
-      <c r="C27" s="10" t="s">
+      <c r="B27" s="6">
+        <v>1</v>
+      </c>
+      <c r="C27" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9">
-        <v>1</v>
-      </c>
-      <c r="K27" s="11">
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6">
+        <v>1</v>
+      </c>
+      <c r="K27" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="20"/>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="25"/>
       <c r="B28" s="4">
         <v>2</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="34"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="3"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4">
@@ -1613,21 +1659,21 @@
       <c r="J28" s="4">
         <v>1</v>
       </c>
-      <c r="K28" s="13">
+      <c r="K28" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="20"/>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
       <c r="B29" s="4">
         <v>3</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="34"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="3"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4">
@@ -1636,140 +1682,113 @@
       <c r="J29" s="4">
         <v>1</v>
       </c>
-      <c r="K29" s="13">
+      <c r="K29" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A30" s="19"/>
-      <c r="B30" s="15">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="26"/>
+      <c r="B30" s="9">
         <v>4</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15">
-        <v>1</v>
-      </c>
-      <c r="I30" s="15">
-        <v>1</v>
-      </c>
-      <c r="J30" s="15">
-        <v>2</v>
-      </c>
-      <c r="K30" s="17">
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9">
+        <v>1</v>
+      </c>
+      <c r="I30" s="9">
+        <v>1</v>
+      </c>
+      <c r="J30" s="9">
+        <v>2</v>
+      </c>
+      <c r="K30" s="10">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="40"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="40"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="41"/>
-    </row>
-    <row r="33" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A33" s="40"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="41"/>
-    </row>
-    <row r="34" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A34" s="40"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="44" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="19"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="19"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="19"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="G34" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="H34" s="28" t="s">
+      <c r="H34" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I34" s="28" t="s">
+      <c r="I34" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="J34" s="28" t="s">
+      <c r="J34" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="K34" s="30" t="s">
+      <c r="K34" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="L34" s="41"/>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="22" t="s">
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="9">
-        <v>1</v>
-      </c>
-      <c r="C35" s="10" t="s">
+      <c r="B35" s="6">
+        <v>1</v>
+      </c>
+      <c r="C35" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="36" t="s">
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9">
-        <v>1</v>
-      </c>
-      <c r="K35" s="11">
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6">
+        <v>1</v>
+      </c>
+      <c r="K35" s="7">
         <v>4</v>
       </c>
       <c r="L35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="23"/>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="35"/>
       <c r="B36" s="4">
         <v>2</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="37"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4">
@@ -1778,24 +1797,24 @@
       <c r="J36" s="4">
         <v>1</v>
       </c>
-      <c r="K36" s="13">
+      <c r="K36" s="8">
         <v>5</v>
       </c>
       <c r="L36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="23"/>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
       <c r="B37" s="4">
         <v>3</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="37"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4">
         <v>1</v>
@@ -1806,81 +1825,81 @@
       <c r="J37" s="4">
         <v>2</v>
       </c>
-      <c r="K37" s="13">
+      <c r="K37" s="8">
         <v>8</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A38" s="24"/>
-      <c r="B38" s="15">
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="36"/>
+      <c r="B38" s="9">
         <v>4</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="15">
-        <v>1</v>
-      </c>
-      <c r="H38" s="15">
-        <v>1</v>
-      </c>
-      <c r="I38" s="15">
-        <v>2</v>
-      </c>
-      <c r="J38" s="15">
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="9">
+        <v>1</v>
+      </c>
+      <c r="H38" s="9">
+        <v>1</v>
+      </c>
+      <c r="I38" s="9">
+        <v>2</v>
+      </c>
+      <c r="J38" s="9">
         <v>3</v>
       </c>
-      <c r="K38" s="17">
+      <c r="K38" s="10">
         <v>12</v>
       </c>
       <c r="L38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="22" t="s">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="9">
-        <v>1</v>
-      </c>
-      <c r="C39" s="10" t="s">
+      <c r="B39" s="6">
+        <v>1</v>
+      </c>
+      <c r="C39" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="25" t="s">
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9">
-        <v>1</v>
-      </c>
-      <c r="J39" s="9">
-        <v>1</v>
-      </c>
-      <c r="K39" s="11">
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6">
+        <v>1</v>
+      </c>
+      <c r="J39" s="6">
+        <v>1</v>
+      </c>
+      <c r="K39" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="23"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="35"/>
       <c r="B40" s="4">
         <v>2</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="6"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="32"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4">
@@ -1889,21 +1908,21 @@
       <c r="J40" s="4">
         <v>2</v>
       </c>
-      <c r="K40" s="13">
+      <c r="K40" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
-      <c r="A41" s="23"/>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="35"/>
       <c r="B41" s="4">
         <v>3</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="6"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="32"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4">
         <v>1</v>
@@ -1914,195 +1933,195 @@
       <c r="J41" s="4">
         <v>2</v>
       </c>
-      <c r="K41" s="13">
+      <c r="K41" s="8">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A42" s="24"/>
-      <c r="B42" s="15">
+    <row r="42" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="36"/>
+      <c r="B42" s="9">
         <v>4</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="15">
-        <v>1</v>
-      </c>
-      <c r="H42" s="15">
-        <v>1</v>
-      </c>
-      <c r="I42" s="15">
-        <v>2</v>
-      </c>
-      <c r="J42" s="15">
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="9">
+        <v>1</v>
+      </c>
+      <c r="H42" s="9">
+        <v>1</v>
+      </c>
+      <c r="I42" s="9">
+        <v>2</v>
+      </c>
+      <c r="J42" s="9">
         <v>3</v>
       </c>
-      <c r="K42" s="17">
+      <c r="K42" s="10">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="8" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="9">
-        <v>1</v>
-      </c>
-      <c r="C43" s="10" t="s">
+      <c r="B43" s="6">
+        <v>1</v>
+      </c>
+      <c r="C43" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="33" t="s">
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9">
-        <v>1</v>
-      </c>
-      <c r="J43" s="9">
-        <v>1</v>
-      </c>
-      <c r="K43" s="11">
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6">
+        <v>1</v>
+      </c>
+      <c r="J43" s="6">
+        <v>1</v>
+      </c>
+      <c r="K43" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A44" s="14"/>
-      <c r="B44" s="15">
-        <v>2</v>
-      </c>
-      <c r="C44" s="16" t="s">
+    <row r="44" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="23"/>
+      <c r="B44" s="9">
+        <v>2</v>
+      </c>
+      <c r="C44" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15">
-        <v>1</v>
-      </c>
-      <c r="I44" s="15">
-        <v>1</v>
-      </c>
-      <c r="J44" s="15">
-        <v>1</v>
-      </c>
-      <c r="K44" s="17">
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9">
+        <v>1</v>
+      </c>
+      <c r="I44" s="9">
+        <v>1</v>
+      </c>
+      <c r="J44" s="9">
+        <v>1</v>
+      </c>
+      <c r="K44" s="10">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
-      <c r="A45" s="18" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="9">
-        <v>1</v>
-      </c>
-      <c r="C45" s="10" t="s">
+      <c r="B45" s="6">
+        <v>1</v>
+      </c>
+      <c r="C45" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A46" s="19"/>
-      <c r="B46" s="15">
-        <v>2</v>
-      </c>
-      <c r="C46" s="16" t="s">
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="26"/>
+      <c r="B46" s="9">
+        <v>2</v>
+      </c>
+      <c r="C46" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="17"/>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="22" t="s">
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="10"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="23"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="35"/>
       <c r="B48" s="4">
         <v>2</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="34"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="3"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4">
         <v>1</v>
       </c>
-      <c r="K48" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A49" s="24"/>
-      <c r="B49" s="15">
+      <c r="K48" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="36"/>
+      <c r="B49" s="9">
         <v>3</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15">
-        <v>1</v>
-      </c>
-      <c r="K49" s="17">
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9">
+        <v>1</v>
+      </c>
+      <c r="K49" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A50" s="27" t="s">
+    <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="28">
+      <c r="B50" s="13">
         <v>1</v>
       </c>
       <c r="C50" s="29" t="s">
@@ -2110,22 +2129,22 @@
       </c>
       <c r="D50" s="29"/>
       <c r="E50" s="29"/>
-      <c r="F50" s="35" t="s">
+      <c r="F50" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G50" s="28"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="28"/>
-      <c r="J50" s="28"/>
-      <c r="K50" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A51" s="27" t="s">
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="28">
+      <c r="B51" s="13">
         <v>1</v>
       </c>
       <c r="C51" s="29" t="s">
@@ -2133,29 +2152,56 @@
       </c>
       <c r="D51" s="29"/>
       <c r="E51" s="29"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="28"/>
-      <c r="H51" s="28"/>
-      <c r="I51" s="28"/>
-      <c r="J51" s="28">
-        <v>1</v>
-      </c>
-      <c r="K51" s="30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11">
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13">
+        <v>1</v>
+      </c>
+      <c r="K51" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="C51:E51"/>
     <mergeCell ref="C52:E52"/>
@@ -2167,30 +2213,19 @@
     <mergeCell ref="C46:E46"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="C48:E48"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C49:E49"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C16:E16"/>
@@ -2198,22 +2233,6 @@
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2221,24 +2240,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>